<commit_message>
add ontology mappings to metadata
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@80035 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/Microbiome/doc/microbiome_terms.xlsx
+++ b/Load/src/ontology/Microbiome/doc/microbiome_terms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="9560" tabRatio="625" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="2020" yWindow="5420" windowWidth="29100" windowHeight="14100" tabRatio="625" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="IRI mappings" sheetId="13" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="microbiome terms" sheetId="14" r:id="rId6"/>
     <sheet name="term need imports" sheetId="15" r:id="rId7"/>
     <sheet name="ontology mapping" sheetId="16" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11041" uniqueCount="2730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11084" uniqueCount="2738">
   <si>
     <t>Name</t>
   </si>
@@ -8181,9 +8182,6 @@
     <t>add to Eupath under process</t>
   </si>
   <si>
-    <t>consult with ENVO developers, or add built environment information to Eupath under ICE</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/ENVO_00000070</t>
   </si>
   <si>
@@ -8193,9 +8191,6 @@
     <t>add to Eupath under ICE</t>
   </si>
   <si>
-    <t>how about clarifying it is child diet</t>
-  </si>
-  <si>
     <t>how about clarifying it is child diet (by month)</t>
   </si>
   <si>
@@ -8233,6 +8228,36 @@
   </si>
   <si>
     <t>investigation title</t>
+  </si>
+  <si>
+    <t>Unclear terms</t>
+  </si>
+  <si>
+    <t>terms need definitions</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33281</t>
+  </si>
+  <si>
+    <t>antimicrobial agent</t>
+  </si>
+  <si>
+    <t>mapped term label</t>
+  </si>
+  <si>
+    <t>mapped term IRI</t>
+  </si>
+  <si>
+    <t>labour and delivery / baby's delivery</t>
+  </si>
+  <si>
+    <t>child diet</t>
+  </si>
+  <si>
+    <t>child diet by month</t>
+  </si>
+  <si>
+    <t>how about clarifying it is child diet, add under  http://www.ebi.ac.uk/efo/EFO_0002755 diet, (term need to import)</t>
   </si>
 </sst>
 </file>
@@ -8945,7 +8970,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="333">
+  <cellStyleXfs count="356">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9279,6 +9304,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -9400,7 +9448,7 @@
     <xf numFmtId="0" fontId="24" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="333">
+  <cellStyles count="356">
     <cellStyle name="20% - Accent1" xfId="208" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="212" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="216" builtinId="38" customBuiltin="1"/>
@@ -9710,6 +9758,29 @@
     <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="196" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="192" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="193" builtinId="17" customBuiltin="1"/>
@@ -44221,18 +44292,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:XFD69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.6640625" customWidth="1"/>
-    <col min="7" max="7" width="6.5" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="42.5" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="41.1640625" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44258,6 +44333,12 @@
         <v>2698</v>
       </c>
       <c r="H1" t="s">
+        <v>2733</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2732</v>
+      </c>
+      <c r="J1" t="s">
         <v>1250</v>
       </c>
     </row>
@@ -44271,11 +44352,11 @@
       <c r="D2" t="s">
         <v>1226</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>1749</v>
+      <c r="F2" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2700</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -44291,11 +44372,11 @@
       <c r="D3" t="s">
         <v>1709</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>1774</v>
+      <c r="F3" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2700</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -44311,11 +44392,11 @@
       <c r="D4" t="s">
         <v>2449</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>1774</v>
+      <c r="F4" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2700</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -44331,11 +44412,17 @@
       <c r="D5" t="s">
         <v>2447</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>1774</v>
+      <c r="F5" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2730</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2731</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -44348,19 +44435,22 @@
       <c r="C6" t="s">
         <v>1176</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>2453</v>
       </c>
       <c r="E6" t="s">
         <v>1710</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>1774</v>
+      <c r="F6" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2700</v>
       </c>
       <c r="I6" s="5" t="s">
+        <v>2734</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>2711</v>
       </c>
     </row>
@@ -44380,21 +44470,17 @@
       <c r="F7" t="s">
         <v>1758</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>1749</v>
+      <c r="G7" t="s">
+        <v>2700</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>1758</v>
+        <v>2712</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>2712</v>
-      </c>
-      <c r="J7" s="10" t="s">
         <v>2713</v>
       </c>
-      <c r="K7" s="10" t="s">
-        <v>2714</v>
-      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
@@ -44406,19 +44492,16 @@
       <c r="D8" t="s">
         <v>1234</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>1758</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="10" t="s">
-        <v>2549</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>1234</v>
-      </c>
+      <c r="G8" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
@@ -44427,20 +44510,23 @@
       <c r="B9" t="s">
         <v>2636</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>1116</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>1758</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>2715</v>
+      <c r="G9" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="5" t="s">
+        <v>1116</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="K9" s="10" t="s">
+        <v>2714</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
@@ -44455,12 +44541,13 @@
       <c r="D10" t="s">
         <v>2693</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>1774</v>
-      </c>
+      <c r="F10" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
@@ -44475,12 +44562,13 @@
       <c r="D11" t="s">
         <v>2451</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>1774</v>
-      </c>
+      <c r="F11" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
@@ -44495,16 +44583,20 @@
       <c r="D12" t="s">
         <v>1277</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>1774</v>
-      </c>
+      <c r="F12" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>2716</v>
+        <v>2735</v>
       </c>
       <c r="J12" s="5"/>
+      <c r="K12" s="5" t="s">
+        <v>2737</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
@@ -44519,16 +44611,20 @@
       <c r="D13" t="s">
         <v>2439</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>1774</v>
-      </c>
+      <c r="F13" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>2717</v>
+        <v>2736</v>
       </c>
       <c r="J13" s="5"/>
+      <c r="K13" s="5" t="s">
+        <v>2715</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
@@ -44543,17 +44639,17 @@
       <c r="E14" t="s">
         <v>1380</v>
       </c>
-      <c r="F14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>1774</v>
-      </c>
+      <c r="F14" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="10" t="s">
+        <v>1774</v>
+      </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11">
@@ -44569,19 +44665,22 @@
       <c r="D15" t="s">
         <v>1713</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>1749</v>
+      <c r="F15" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2700</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I15" s="10"/>
+        <v>2716</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>2717</v>
+      </c>
       <c r="J15" s="10" t="s">
-        <v>2718</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>2719</v>
-      </c>
+        <v>1774</v>
+      </c>
+      <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
@@ -44596,22 +44695,22 @@
       <c r="E16" t="s">
         <v>1584</v>
       </c>
-      <c r="F16" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>1749</v>
+      <c r="F16" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2700</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I16" s="10"/>
+        <v>2718</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>2719</v>
+      </c>
       <c r="J16" s="10" t="s">
-        <v>2720</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>2721</v>
-      </c>
+        <v>1774</v>
+      </c>
+      <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
@@ -44626,22 +44725,22 @@
       <c r="E17" t="s">
         <v>1585</v>
       </c>
-      <c r="F17" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>1749</v>
+      <c r="F17" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2700</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I17" s="10"/>
+        <v>2720</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>2721</v>
+      </c>
       <c r="J17" s="10" t="s">
-        <v>2722</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>2723</v>
-      </c>
+        <v>1774</v>
+      </c>
+      <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
@@ -44653,17 +44752,20 @@
       <c r="D18" t="s">
         <v>1080</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>1758</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>2715</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="G18" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10" t="s">
+        <v>1758</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>2714</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
@@ -44678,22 +44780,22 @@
       <c r="E19" t="s">
         <v>1586</v>
       </c>
-      <c r="F19" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>1749</v>
+      <c r="F19" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2700</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I19" s="10"/>
+        <v>2722</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>945</v>
+      </c>
       <c r="J19" s="10" t="s">
-        <v>2724</v>
-      </c>
-      <c r="K19" s="10" t="s">
-        <v>945</v>
-      </c>
+        <v>1774</v>
+      </c>
+      <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
@@ -44708,10 +44810,13 @@
       <c r="D20" t="s">
         <v>2454</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H20" s="5" t="s">
+      <c r="F20" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G20" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44731,10 +44836,13 @@
       <c r="E21" t="s">
         <v>1719</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H21" s="5" t="s">
+      <c r="F21" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G21" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44748,10 +44856,13 @@
       <c r="D22" t="s">
         <v>1089</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H22" s="11" t="s">
+      <c r="F22" s="11" t="s">
+        <v>1758</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J22" s="11" t="s">
         <v>1758</v>
       </c>
     </row>
@@ -44768,13 +44879,13 @@
       <c r="E23" t="s">
         <v>1592</v>
       </c>
-      <c r="F23" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H23" s="11" t="s">
+      <c r="F23" s="11" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G23" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J23" s="11" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44791,13 +44902,13 @@
       <c r="E24" t="s">
         <v>1256</v>
       </c>
-      <c r="F24" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H24" s="10" t="s">
+      <c r="F24" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J24" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44814,13 +44925,13 @@
       <c r="E25" t="s">
         <v>1262</v>
       </c>
-      <c r="F25" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H25" s="10" t="s">
+      <c r="F25" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J25" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44837,13 +44948,13 @@
       <c r="E26" t="s">
         <v>1266</v>
       </c>
-      <c r="F26" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H26" s="10" t="s">
+      <c r="F26" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J26" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44860,13 +44971,13 @@
       <c r="E27" t="s">
         <v>1268</v>
       </c>
-      <c r="F27" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H27" s="10" t="s">
+      <c r="F27" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G27" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J27" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44883,13 +44994,13 @@
       <c r="E28" t="s">
         <v>1274</v>
       </c>
-      <c r="F28" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H28" s="10" t="s">
+      <c r="F28" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G28" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J28" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44906,13 +45017,13 @@
       <c r="E29" t="s">
         <v>1276</v>
       </c>
-      <c r="F29" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H29" s="10" t="s">
+      <c r="F29" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G29" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J29" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44929,13 +45040,13 @@
       <c r="E30" t="s">
         <v>1282</v>
       </c>
-      <c r="F30" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H30" s="10" t="s">
+      <c r="F30" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G30" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J30" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -44949,14 +45060,17 @@
       <c r="D31" t="s">
         <v>1077</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H31" s="10" t="s">
+      <c r="F31" s="10" t="s">
         <v>1758</v>
       </c>
-      <c r="I31" s="10" t="s">
-        <v>2715</v>
+      <c r="G31" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>1758</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>2714</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -44975,15 +45089,15 @@
       <c r="F32" t="s">
         <v>1774</v>
       </c>
-      <c r="G32" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I32" s="10"/>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="G32" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>2547</v>
       </c>
@@ -44999,15 +45113,15 @@
       <c r="F33" t="s">
         <v>1774</v>
       </c>
-      <c r="G33" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I33" s="10"/>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="G33" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -45023,14 +45137,14 @@
       <c r="F34" t="s">
         <v>1774</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="G34" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>2551</v>
       </c>
@@ -45040,14 +45154,17 @@
       <c r="D35" t="s">
         <v>1236</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H35" s="10" t="s">
+      <c r="F35" s="10" t="s">
         <v>1758</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="G35" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>2518</v>
       </c>
@@ -45060,14 +45177,17 @@
       <c r="D36" t="s">
         <v>2692</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="F36" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G36" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>2521</v>
       </c>
@@ -45077,14 +45197,17 @@
       <c r="D37" t="s">
         <v>1180</v>
       </c>
-      <c r="G37" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="F37" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G37" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>2522</v>
       </c>
@@ -45094,14 +45217,17 @@
       <c r="D38" t="s">
         <v>1196</v>
       </c>
-      <c r="G38" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="F38" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G38" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>2520</v>
       </c>
@@ -45114,14 +45240,17 @@
       <c r="D39" t="s">
         <v>2456</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="F39" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G39" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>2519</v>
       </c>
@@ -45134,14 +45263,17 @@
       <c r="D40" t="s">
         <v>2455</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="F40" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G40" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>2529</v>
       </c>
@@ -45154,14 +45286,17 @@
       <c r="D41" t="s">
         <v>2463</v>
       </c>
-      <c r="G41" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="F41" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G41" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>2530</v>
       </c>
@@ -45174,14 +45309,17 @@
       <c r="D42" t="s">
         <v>2464</v>
       </c>
-      <c r="G42" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="F42" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G42" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -45194,17 +45332,17 @@
       <c r="E43" t="s">
         <v>1255</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="10" t="s">
         <v>1758</v>
       </c>
-      <c r="G43" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H43" s="10" t="s">
+      <c r="G43" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J43" s="10" t="s">
         <v>1758</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>2531</v>
       </c>
@@ -45217,14 +45355,17 @@
       <c r="D44" t="s">
         <v>2465</v>
       </c>
-      <c r="G44" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="F44" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G44" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>2532</v>
       </c>
@@ -45237,14 +45378,17 @@
       <c r="D45" t="s">
         <v>2466</v>
       </c>
-      <c r="G45" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="F45" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G45" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>2523</v>
       </c>
@@ -45260,16 +45404,19 @@
       <c r="E46" t="s">
         <v>1716</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="F46" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G46" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H46" s="5"/>
+      <c r="J46" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>2524</v>
       </c>
@@ -45285,16 +45432,19 @@
       <c r="E47" t="s">
         <v>1717</v>
       </c>
-      <c r="G47" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="F47" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G47" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H47" s="5"/>
+      <c r="J47" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K47" s="5"/>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>2525</v>
       </c>
@@ -45310,14 +45460,17 @@
       <c r="E48" t="s">
         <v>1718</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
+      <c r="F48" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G48" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H48" s="5"/>
+      <c r="J48" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
@@ -45332,19 +45485,19 @@
       <c r="E49" t="s">
         <v>1462</v>
       </c>
-      <c r="F49" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>2715</v>
-      </c>
-      <c r="J49" s="10"/>
+      <c r="F49" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G49" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="J49" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>2714</v>
+      </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
@@ -45359,10 +45512,13 @@
       <c r="E50" t="s">
         <v>2691</v>
       </c>
-      <c r="G50" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H50" s="10" t="s">
+      <c r="F50" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G50" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J50" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -45379,10 +45535,13 @@
       <c r="D51" t="s">
         <v>2467</v>
       </c>
-      <c r="G51" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H51" s="5" t="s">
+      <c r="F51" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G51" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J51" s="5" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -45396,10 +45555,13 @@
       <c r="D52" t="s">
         <v>1160</v>
       </c>
-      <c r="G52" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H52" s="10" t="s">
+      <c r="F52" s="10" t="s">
+        <v>1758</v>
+      </c>
+      <c r="G52" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J52" s="10" t="s">
         <v>1758</v>
       </c>
     </row>
@@ -45413,10 +45575,13 @@
       <c r="D53" t="s">
         <v>1148</v>
       </c>
-      <c r="G53" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H53" s="10" t="s">
+      <c r="F53" s="10" t="s">
+        <v>1758</v>
+      </c>
+      <c r="G53" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J53" s="10" t="s">
         <v>1758</v>
       </c>
     </row>
@@ -45433,10 +45598,13 @@
       <c r="D54" t="s">
         <v>2468</v>
       </c>
-      <c r="G54" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H54" s="5" t="s">
+      <c r="F54" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G54" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -45453,10 +45621,13 @@
       <c r="D55" t="s">
         <v>2470</v>
       </c>
-      <c r="G55" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H55" s="5" t="s">
+      <c r="F55" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G55" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J55" s="5" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -45473,10 +45644,13 @@
       <c r="D56" t="s">
         <v>1230</v>
       </c>
-      <c r="G56" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H56" s="5" t="s">
+      <c r="F56" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G56" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J56" s="5" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -45490,10 +45664,13 @@
       <c r="D57" t="s">
         <v>1208</v>
       </c>
-      <c r="G57" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H57" s="5" t="s">
+      <c r="F57" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G57" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J57" s="5" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -45507,13 +45684,16 @@
       <c r="D58" t="s">
         <v>1106</v>
       </c>
-      <c r="G58" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H58" s="10" t="s">
+      <c r="F58" s="10" t="s">
         <v>1758</v>
       </c>
-      <c r="I58" s="10"/>
+      <c r="G58" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J58" s="10" t="s">
+        <v>1758</v>
+      </c>
+      <c r="K58" s="10"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
@@ -45528,14 +45708,17 @@
       <c r="D59" t="s">
         <v>2471</v>
       </c>
-      <c r="G59" s="5" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>2725</v>
+      <c r="F59" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G59" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K59" s="5" t="s">
+        <v>2723</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -45548,14 +45731,17 @@
       <c r="D60" t="s">
         <v>1252</v>
       </c>
-      <c r="G60" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H60" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I60" s="10" t="s">
-        <v>2726</v>
+      <c r="F60" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G60" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J60" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K60" s="10" t="s">
+        <v>2724</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -45568,20 +45754,23 @@
       <c r="D61" t="s">
         <v>1198</v>
       </c>
-      <c r="G61" s="10" t="s">
-        <v>1749</v>
+      <c r="F61" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G61" t="s">
+        <v>2700</v>
       </c>
       <c r="H61" s="10" t="s">
-        <v>1774</v>
+        <v>2726</v>
       </c>
       <c r="I61" s="10" t="s">
         <v>2727</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>2728</v>
+        <v>1774</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>2729</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -45597,13 +45786,13 @@
       <c r="E62" t="s">
         <v>1572</v>
       </c>
-      <c r="F62" t="s">
-        <v>1774</v>
-      </c>
-      <c r="G62" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H62" s="10" t="s">
+      <c r="F62" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G62" t="s">
+        <v>2700</v>
+      </c>
+      <c r="J62" s="10" t="s">
         <v>1774</v>
       </c>
     </row>
@@ -45627,13 +45816,13 @@
         <v>2700</v>
       </c>
       <c r="H63" t="s">
+        <v>2708</v>
+      </c>
+      <c r="J63" t="s">
         <v>2707</v>
       </c>
-      <c r="I63" t="s">
+      <c r="K63" t="s">
         <v>2709</v>
-      </c>
-      <c r="J63" t="s">
-        <v>2708</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -45655,14 +45844,14 @@
       <c r="G64" t="s">
         <v>2700</v>
       </c>
-      <c r="I64" t="s">
+      <c r="H64" t="s">
+        <v>2704</v>
+      </c>
+      <c r="K64" t="s">
         <v>2703</v>
       </c>
-      <c r="J64" t="s">
-        <v>2704</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" t="s">
         <v>2526</v>
       </c>
@@ -45678,11 +45867,11 @@
       <c r="G65" t="s">
         <v>2700</v>
       </c>
-      <c r="H65" t="s">
+      <c r="J65" t="s">
         <v>2710</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>2555</v>
       </c>
@@ -45698,11 +45887,11 @@
       <c r="G66" t="s">
         <v>2700</v>
       </c>
-      <c r="H66" t="s">
+      <c r="J66" t="s">
         <v>2705</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>1033</v>
       </c>
@@ -45721,11 +45910,11 @@
       <c r="G67" t="s">
         <v>2700</v>
       </c>
-      <c r="H67" t="s">
+      <c r="J67" t="s">
         <v>2706</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>1075</v>
       </c>
@@ -45741,14 +45930,14 @@
       <c r="G68" t="s">
         <v>2700</v>
       </c>
-      <c r="H68" t="s">
+      <c r="J68" t="s">
         <v>2701</v>
       </c>
-      <c r="I68" t="s">
+      <c r="K68" t="s">
         <v>2702</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>2546</v>
       </c>
@@ -45767,11 +45956,11 @@
       <c r="G69" t="s">
         <v>2700</v>
       </c>
-      <c r="H69" t="s">
+      <c r="J69" t="s">
         <v>2705</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -45788,7 +45977,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>2497</v>
       </c>
@@ -45799,7 +45988,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>2501</v>
       </c>
@@ -45810,7 +45999,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:11">
       <c r="A73" t="s">
         <v>910</v>
       </c>
@@ -45827,7 +46016,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -45844,7 +46033,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:11">
       <c r="A75" t="s">
         <v>2544</v>
       </c>
@@ -45855,7 +46044,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:11">
       <c r="A76" t="s">
         <v>149</v>
       </c>
@@ -45872,7 +46061,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:11">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -45889,7 +46078,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:11">
       <c r="A78" t="s">
         <v>161</v>
       </c>
@@ -45906,7 +46095,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:11">
       <c r="A79" t="s">
         <v>164</v>
       </c>
@@ -45923,7 +46112,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:11">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -47281,7 +47470,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:10">
       <c r="A161" t="s">
         <v>665</v>
       </c>
@@ -47298,7 +47487,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:10">
       <c r="A162" t="s">
         <v>2560</v>
       </c>
@@ -47309,7 +47498,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:10">
       <c r="A163" t="s">
         <v>344</v>
       </c>
@@ -47326,7 +47515,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:10">
       <c r="A164" t="s">
         <v>347</v>
       </c>
@@ -47343,7 +47532,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:10">
       <c r="A165" t="s">
         <v>961</v>
       </c>
@@ -47360,7 +47549,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:10">
       <c r="A166" t="s">
         <v>356</v>
       </c>
@@ -47377,7 +47566,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:10">
       <c r="A167" t="s">
         <v>362</v>
       </c>
@@ -47394,7 +47583,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:10">
       <c r="A168" t="s">
         <v>365</v>
       </c>
@@ -47411,7 +47600,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:10">
       <c r="A169" t="s">
         <v>368</v>
       </c>
@@ -47428,7 +47617,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:10">
       <c r="A170" t="s">
         <v>371</v>
       </c>
@@ -47445,7 +47634,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:10">
       <c r="A171" t="s">
         <v>913</v>
       </c>
@@ -47462,9 +47651,9 @@
         <v>1774</v>
       </c>
       <c r="G171" s="10"/>
-      <c r="H171" s="10"/>
-    </row>
-    <row r="172" spans="1:8">
+      <c r="J171" s="10"/>
+    </row>
+    <row r="172" spans="1:10">
       <c r="A172" t="s">
         <v>2491</v>
       </c>
@@ -47481,7 +47670,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:10">
       <c r="A173" t="s">
         <v>979</v>
       </c>
@@ -47498,7 +47687,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:10">
       <c r="A174" t="s">
         <v>377</v>
       </c>
@@ -47515,7 +47704,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:10">
       <c r="A175" t="s">
         <v>380</v>
       </c>
@@ -47532,7 +47721,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:10">
       <c r="A176" t="s">
         <v>383</v>
       </c>
@@ -47815,7 +48004,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:11">
       <c r="A193" t="s">
         <v>410</v>
       </c>
@@ -47832,7 +48021,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:11">
       <c r="A194" t="s">
         <v>47</v>
       </c>
@@ -47849,9 +48038,9 @@
         <v>1774</v>
       </c>
       <c r="G194" s="10"/>
-      <c r="H194" s="10"/>
-    </row>
-    <row r="195" spans="1:9">
+      <c r="J194" s="10"/>
+    </row>
+    <row r="195" spans="1:11">
       <c r="A195" t="s">
         <v>50</v>
       </c>
@@ -47868,9 +48057,9 @@
         <v>1774</v>
       </c>
       <c r="G195" s="10"/>
-      <c r="H195" s="10"/>
-    </row>
-    <row r="196" spans="1:9">
+      <c r="J195" s="10"/>
+    </row>
+    <row r="196" spans="1:11">
       <c r="A196" t="s">
         <v>65</v>
       </c>
@@ -47887,9 +48076,9 @@
         <v>1774</v>
       </c>
       <c r="G196" s="10"/>
-      <c r="H196" s="10"/>
-    </row>
-    <row r="197" spans="1:9">
+      <c r="J196" s="10"/>
+    </row>
+    <row r="197" spans="1:11">
       <c r="A197" t="s">
         <v>56</v>
       </c>
@@ -47906,9 +48095,9 @@
         <v>1774</v>
       </c>
       <c r="G197" s="10"/>
-      <c r="H197" s="10"/>
-    </row>
-    <row r="198" spans="1:9">
+      <c r="J197" s="10"/>
+    </row>
+    <row r="198" spans="1:11">
       <c r="A198" t="s">
         <v>68</v>
       </c>
@@ -47925,9 +48114,9 @@
         <v>1774</v>
       </c>
       <c r="G198" s="10"/>
-      <c r="H198" s="10"/>
-    </row>
-    <row r="199" spans="1:9">
+      <c r="J198" s="10"/>
+    </row>
+    <row r="199" spans="1:11">
       <c r="A199" t="s">
         <v>77</v>
       </c>
@@ -47944,9 +48133,9 @@
         <v>1774</v>
       </c>
       <c r="G199" s="10"/>
-      <c r="H199" s="10"/>
-    </row>
-    <row r="200" spans="1:9">
+      <c r="J199" s="10"/>
+    </row>
+    <row r="200" spans="1:11">
       <c r="A200" t="s">
         <v>80</v>
       </c>
@@ -47963,9 +48152,9 @@
         <v>1774</v>
       </c>
       <c r="G200" s="10"/>
-      <c r="H200" s="10"/>
-    </row>
-    <row r="201" spans="1:9">
+      <c r="J200" s="10"/>
+    </row>
+    <row r="201" spans="1:11">
       <c r="A201" t="s">
         <v>86</v>
       </c>
@@ -47982,7 +48171,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:11">
       <c r="A202" t="s">
         <v>89</v>
       </c>
@@ -47999,7 +48188,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:11">
       <c r="A203" t="s">
         <v>92</v>
       </c>
@@ -48016,7 +48205,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:11">
       <c r="A204" t="s">
         <v>95</v>
       </c>
@@ -48033,7 +48222,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:11">
       <c r="A205" t="s">
         <v>98</v>
       </c>
@@ -48050,10 +48239,10 @@
         <v>1774</v>
       </c>
       <c r="G205" s="10"/>
-      <c r="H205" s="10"/>
-      <c r="I205" s="10"/>
-    </row>
-    <row r="206" spans="1:9">
+      <c r="J205" s="10"/>
+      <c r="K205" s="10"/>
+    </row>
+    <row r="206" spans="1:11">
       <c r="A206" t="s">
         <v>101</v>
       </c>
@@ -48070,10 +48259,10 @@
         <v>1774</v>
       </c>
       <c r="G206" s="10"/>
-      <c r="H206" s="10"/>
-      <c r="I206" s="10"/>
-    </row>
-    <row r="207" spans="1:9">
+      <c r="J206" s="10"/>
+      <c r="K206" s="10"/>
+    </row>
+    <row r="207" spans="1:11">
       <c r="A207" t="s">
         <v>104</v>
       </c>
@@ -48090,10 +48279,10 @@
         <v>1774</v>
       </c>
       <c r="G207" s="10"/>
-      <c r="H207" s="10"/>
-      <c r="I207" s="10"/>
-    </row>
-    <row r="208" spans="1:9">
+      <c r="J207" s="10"/>
+      <c r="K207" s="10"/>
+    </row>
+    <row r="208" spans="1:11">
       <c r="A208" t="s">
         <v>107</v>
       </c>
@@ -48110,10 +48299,10 @@
         <v>1774</v>
       </c>
       <c r="G208" s="10"/>
-      <c r="H208" s="10"/>
-      <c r="I208" s="10"/>
-    </row>
-    <row r="209" spans="1:9">
+      <c r="J208" s="10"/>
+      <c r="K208" s="10"/>
+    </row>
+    <row r="209" spans="1:11">
       <c r="A209" t="s">
         <v>113</v>
       </c>
@@ -48130,10 +48319,10 @@
         <v>1774</v>
       </c>
       <c r="G209" s="10"/>
-      <c r="H209" s="10"/>
-      <c r="I209" s="10"/>
-    </row>
-    <row r="210" spans="1:9">
+      <c r="J209" s="10"/>
+      <c r="K209" s="10"/>
+    </row>
+    <row r="210" spans="1:11">
       <c r="A210" t="s">
         <v>116</v>
       </c>
@@ -48150,10 +48339,10 @@
         <v>1774</v>
       </c>
       <c r="G210" s="10"/>
-      <c r="H210" s="10"/>
-      <c r="I210" s="10"/>
-    </row>
-    <row r="211" spans="1:9">
+      <c r="J210" s="10"/>
+      <c r="K210" s="10"/>
+    </row>
+    <row r="211" spans="1:11">
       <c r="A211" t="s">
         <v>119</v>
       </c>
@@ -48170,10 +48359,10 @@
         <v>1774</v>
       </c>
       <c r="G211" s="10"/>
-      <c r="H211" s="10"/>
-      <c r="I211" s="10"/>
-    </row>
-    <row r="212" spans="1:9">
+      <c r="J211" s="10"/>
+      <c r="K211" s="10"/>
+    </row>
+    <row r="212" spans="1:11">
       <c r="A212" t="s">
         <v>125</v>
       </c>
@@ -48190,7 +48379,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:11">
       <c r="A213" t="s">
         <v>970</v>
       </c>
@@ -48207,7 +48396,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:11">
       <c r="A214" t="s">
         <v>128</v>
       </c>
@@ -48224,7 +48413,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:11">
       <c r="A215" t="s">
         <v>131</v>
       </c>
@@ -48241,7 +48430,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:11">
       <c r="A216" t="s">
         <v>134</v>
       </c>
@@ -48258,7 +48447,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:11">
       <c r="A217" t="s">
         <v>140</v>
       </c>
@@ -48275,9 +48464,9 @@
         <v>1774</v>
       </c>
       <c r="G217" s="10"/>
-      <c r="H217" s="10"/>
-    </row>
-    <row r="218" spans="1:9">
+      <c r="J217" s="10"/>
+    </row>
+    <row r="218" spans="1:11">
       <c r="A218" t="s">
         <v>413</v>
       </c>
@@ -48294,7 +48483,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:11">
       <c r="A219" t="s">
         <v>416</v>
       </c>
@@ -48311,7 +48500,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:11">
       <c r="A220" t="s">
         <v>419</v>
       </c>
@@ -48328,7 +48517,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:11">
       <c r="A221" t="s">
         <v>422</v>
       </c>
@@ -48345,7 +48534,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:11">
       <c r="A222" t="s">
         <v>425</v>
       </c>
@@ -48362,7 +48551,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:11">
       <c r="A223" t="s">
         <v>428</v>
       </c>
@@ -48379,7 +48568,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:11">
       <c r="A224" t="s">
         <v>431</v>
       </c>
@@ -52040,4 +52229,64 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>2728</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>2729</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>2439</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added information provided by Dan
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@80074 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/Microbiome/doc/microbiome_terms.xlsx
+++ b/Load/src/ontology/Microbiome/doc/microbiome_terms.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="5420" windowWidth="29100" windowHeight="14100" tabRatio="625" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="7160" yWindow="4700" windowWidth="25600" windowHeight="14420" tabRatio="625" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="IRI mappings" sheetId="13" r:id="rId1"/>
+    <sheet name="IRI mappings(webProtege)" sheetId="13" r:id="rId1"/>
     <sheet name="Todo" sheetId="4" r:id="rId2"/>
     <sheet name="Todo by Dan" sheetId="11" r:id="rId3"/>
     <sheet name="synonym" sheetId="9" r:id="rId4"/>
@@ -15,7 +15,7 @@
     <sheet name="microbiome terms" sheetId="14" r:id="rId6"/>
     <sheet name="term need imports" sheetId="15" r:id="rId7"/>
     <sheet name="ontology mapping" sheetId="16" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="17" r:id="rId9"/>
+    <sheet name="ToDo in ontology" sheetId="17" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11084" uniqueCount="2738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11153" uniqueCount="2815">
   <si>
     <t>Name</t>
   </si>
@@ -8161,12 +8161,6 @@
     <t>comment on investigation</t>
   </si>
   <si>
-    <t>use ontological label</t>
-  </si>
-  <si>
-    <t>add to EuPath under protocol?</t>
-  </si>
-  <si>
     <t>is it same as collection date</t>
   </si>
   <si>
@@ -8191,9 +8185,6 @@
     <t>add to Eupath under ICE</t>
   </si>
   <si>
-    <t>how about clarifying it is child diet (by month)</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/EUPATH_0000494</t>
   </si>
   <si>
@@ -8215,15 +8206,9 @@
     <t>http://purl.obolibrary.org/obo/ENVO_00010483</t>
   </si>
   <si>
-    <t>subject ID?</t>
-  </si>
-  <si>
     <t>surface of sample source?</t>
   </si>
   <si>
-    <t>project title/study title?</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/OBI_0001622</t>
   </si>
   <si>
@@ -8248,23 +8233,269 @@
     <t>mapped term IRI</t>
   </si>
   <si>
-    <t>labour and delivery / baby's delivery</t>
-  </si>
-  <si>
-    <t>child diet</t>
-  </si>
-  <si>
     <t>child diet by month</t>
   </si>
   <si>
-    <t>how about clarifying it is child diet, add under  http://www.ebi.ac.uk/efo/EFO_0002755 diet, (term need to import)</t>
+    <t>environment information</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000493</t>
+  </si>
+  <si>
+    <t>family identifier</t>
+  </si>
+  <si>
+    <t>information of whether family move</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000542</t>
+  </si>
+  <si>
+    <t>location of specimen collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.ebi.ac.uk/efo/EFO_0002755 </t>
+  </si>
+  <si>
+    <t>need import</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_23888/http://www.ebi.ac.uk/efo/EFO_0007010</t>
+  </si>
+  <si>
+    <t>drug/drug use measurement</t>
+  </si>
+  <si>
+    <t>it seems more than one term need to use for describe it.</t>
+  </si>
+  <si>
+    <t>Is this mapping correct? Shall we reverse the mapping for two terms?</t>
+  </si>
+  <si>
+    <t>the description trimmed down, need to check MiXS set to get the full description</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UBERON_0000463</t>
+  </si>
+  <si>
+    <t>organism substance</t>
+  </si>
+  <si>
+    <t>multicellular anatomical structure</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UBERON_0010000</t>
+  </si>
+  <si>
+    <t>common name of organism</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">body habitat behavior </t>
+  </si>
+  <si>
+    <t>add to EuPath under GO:behavior (proposed definition: the general condition of the body as outwardly apparent: any constitutional tendency or weakness)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ERO_0002033</t>
+  </si>
+  <si>
+    <t>family relationship</t>
+  </si>
+  <si>
+    <t>host information</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UBERON_0000105</t>
+  </si>
+  <si>
+    <t>life cycle stage</t>
+  </si>
+  <si>
+    <t>add to Eupath under data item</t>
+  </si>
+  <si>
+    <t>host mass at specimen collection</t>
+  </si>
+  <si>
+    <t>number of child occupants in a household/dwelling?</t>
+  </si>
+  <si>
+    <t>number of human occupants in a household/dwelling?</t>
+  </si>
+  <si>
+    <t>add to EuPath under data item</t>
+  </si>
+  <si>
+    <t>labor and delivery / baby's delivery</t>
+  </si>
+  <si>
+    <t>percent adult occupants in a household/dwelling</t>
+  </si>
+  <si>
+    <t>percent male occupants in a household/dwelling</t>
+  </si>
+  <si>
+    <t>other clinical information?</t>
+  </si>
+  <si>
+    <t>information of class of antibiotics given to mom</t>
+  </si>
+  <si>
+    <t>information of whether antibiotics given to mom</t>
+  </si>
+  <si>
+    <t>information of trimester antibiotics given to mom</t>
+  </si>
+  <si>
+    <t>environmental pets or farm animals information</t>
+  </si>
+  <si>
+    <t>add to Eupath under ICE? Can use 'dwelling animal information' (EUPATH_0000339) [A dwelling information about animal living in a human dwelling.]? Current term is under clinical information. It is means only applied to human.</t>
+  </si>
+  <si>
+    <t>SO:region or ICE?</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0600047</t>
+  </si>
+  <si>
+    <t>sequencing protocol</t>
+  </si>
+  <si>
+    <t>add to EuPath under protocol</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
+  </si>
+  <si>
+    <t>sequencing facility organization</t>
+  </si>
+  <si>
+    <t>investigation summary information</t>
+  </si>
+  <si>
+    <t>identifier of participant under investigation(synonyn: subject identifier)</t>
+  </si>
+  <si>
+    <t>add to Eupath under CRID symbol</t>
+  </si>
+  <si>
+    <t>specimen collection protocol</t>
+  </si>
+  <si>
+    <t>the animal's or human's age counted in days</t>
+  </si>
+  <si>
+    <t>add to Eupath under age since birth measurement datum</t>
+  </si>
+  <si>
+    <t>was the child exposed to antibiotics?</t>
+  </si>
+  <si>
+    <t>information of whether child exposed to antibiotics</t>
+  </si>
+  <si>
+    <t>human clinical information</t>
+  </si>
+  <si>
+    <t>bee colony tetracycline</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Microbiome ontology</t>
+  </si>
+  <si>
+    <t>- update label</t>
+  </si>
+  <si>
+    <t>- update definition</t>
+  </si>
+  <si>
+    <t>- updated URI for mapped ontology terms</t>
+  </si>
+  <si>
+    <t>was the bee colony treated with tetracycline</t>
+  </si>
+  <si>
+    <t>information of whether bee colony treated with tetracycline</t>
+  </si>
+  <si>
+    <t>the number of courses of antibiotics received by the human or animal</t>
+  </si>
+  <si>
+    <t>number of courses of antibiotics given</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000492</t>
+  </si>
+  <si>
+    <t>Child's diet</t>
+  </si>
+  <si>
+    <t>overall, what the main source of nutrition for the child?</t>
+  </si>
+  <si>
+    <t>child's diet</t>
+  </si>
+  <si>
+    <t>need import under 'protocol'</t>
+  </si>
+  <si>
+    <t>add to Eupath under diet</t>
+  </si>
+  <si>
+    <t>not yet</t>
+  </si>
+  <si>
+    <t>Bee larval tetracycline</t>
+  </si>
+  <si>
+    <t>were bee larvae treated with tetracycline?</t>
+  </si>
+  <si>
+    <t>information of whether bee larvae treated with tetracycline</t>
+  </si>
+  <si>
+    <t>Number of courses of antibiotics received by mom prior to delivery</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000497</t>
+  </si>
+  <si>
+    <t>number of courses of antibiotics received by mom prior to delivery</t>
+  </si>
+  <si>
+    <t>Choose samples obtained from the mother, from the child, or both.</t>
+  </si>
+  <si>
+    <t>information of specimen obtained from the mother or chid</t>
+  </si>
+  <si>
+    <t>In which batch were samples sequenced together</t>
+  </si>
+  <si>
+    <t>At which center were samples sequenced</t>
+  </si>
+  <si>
+    <t>sequencing batch information</t>
+  </si>
+  <si>
+    <t>Need check terms in yellow background and hierachy with DAN</t>
+  </si>
+  <si>
+    <t>It is map to age since birth, do we need to specify the age is about host? if so, need to add a new term, (age since birth and is about (age and inheres_in (organism and has_role host role))). The question apply to all host related terms. If might be fine since all terms under 'host information' category.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8594,8 +8825,52 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8853,6 +9128,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -8970,7 +9251,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="356">
+  <cellStyleXfs count="437">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9327,8 +9608,89 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -9447,8 +9809,21 @@
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="356">
+  <cellStyles count="437">
     <cellStyle name="20% - Accent1" xfId="208" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="212" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="216" builtinId="38" customBuiltin="1"/>
@@ -9781,6 +10156,87 @@
     <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="431" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="433" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="435" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="196" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="192" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="193" builtinId="17" customBuiltin="1"/>
@@ -10141,10 +10597,10 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="H73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C69" sqref="C69"/>
+      <selection pane="bottomRight" activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -44265,7 +44721,7 @@
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -44280,6 +44736,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -44292,13 +44749,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K447"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="1.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
@@ -44307,40 +44765,41 @@
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
     <col min="8" max="8" width="41.1640625" customWidth="1"/>
     <col min="9" max="9" width="23.1640625" customWidth="1"/>
-    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="11" max="11" width="22.5" style="120" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="116" customFormat="1" ht="18">
+      <c r="A1" s="116" t="s">
         <v>2685</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="116" t="s">
         <v>2686</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="116" t="s">
         <v>2687</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="116" t="s">
         <v>2699</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="116" t="s">
         <v>2688</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="122" t="s">
         <v>2689</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="116" t="s">
         <v>2698</v>
       </c>
-      <c r="H1" t="s">
-        <v>2733</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2732</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="H1" s="116" t="s">
+        <v>2728</v>
+      </c>
+      <c r="I1" s="116" t="s">
+        <v>2727</v>
+      </c>
+      <c r="J1" s="116" t="s">
         <v>1250</v>
       </c>
+      <c r="K1" s="123"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
@@ -44349,10 +44808,10 @@
       <c r="B2" t="s">
         <v>2591</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="126" t="s">
         <v>1226</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G2" t="s">
@@ -44369,14 +44828,23 @@
       <c r="C3" t="s">
         <v>1248</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>1709</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" t="s">
+        <v>2780</v>
+      </c>
+      <c r="F3" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G3" t="s">
         <v>2700</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1709</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2781</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -44389,14 +44857,23 @@
       <c r="C4" t="s">
         <v>1204</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>2449</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" t="s">
+        <v>2782</v>
+      </c>
+      <c r="F4" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G4" t="s">
         <v>2700</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>2783</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2712</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -44412,17 +44889,20 @@
       <c r="D5" t="s">
         <v>2447</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G5" t="s">
         <v>2700</v>
       </c>
       <c r="H5" t="s">
-        <v>2730</v>
+        <v>2725</v>
       </c>
       <c r="I5" t="s">
-        <v>2731</v>
+        <v>2726</v>
+      </c>
+      <c r="J5" s="125" t="s">
+        <v>2737</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -44441,17 +44921,17 @@
       <c r="E6" t="s">
         <v>1710</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G6" t="s">
         <v>2700</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>2734</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>2711</v>
+        <v>2761</v>
+      </c>
+      <c r="J6" s="94" t="s">
+        <v>2709</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -44467,20 +44947,19 @@
       <c r="E7" t="s">
         <v>1255</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G7" t="s">
         <v>2700</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>2712</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>2713</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="H7" s="94" t="s">
+        <v>2710</v>
+      </c>
+      <c r="I7" s="94" t="s">
+        <v>2711</v>
+      </c>
+      <c r="J7" s="94"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
@@ -44492,16 +44971,16 @@
       <c r="D8" t="s">
         <v>1234</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G8" t="s">
         <v>2700</v>
       </c>
       <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="5"/>
+      <c r="J8" s="125" t="s">
+        <v>2737</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
@@ -44511,9 +44990,9 @@
         <v>2636</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>1116</v>
-      </c>
-      <c r="F9" s="10" t="s">
+        <v>2784</v>
+      </c>
+      <c r="F9" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G9" t="s">
@@ -44521,11 +45000,10 @@
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="5" t="s">
-        <v>1116</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10" t="s">
-        <v>2714</v>
+        <v>2784</v>
+      </c>
+      <c r="J9" s="94" t="s">
+        <v>2712</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -44538,16 +45016,24 @@
       <c r="C10" t="s">
         <v>1190</v>
       </c>
-      <c r="D10" t="s">
-        <v>2693</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="D10" s="5" t="s">
+        <v>2785</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2791</v>
+      </c>
+      <c r="F10" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G10" t="s">
         <v>2700</v>
       </c>
-      <c r="J10" s="10"/>
+      <c r="I10" s="5" t="s">
+        <v>2792</v>
+      </c>
+      <c r="J10" s="94" t="s">
+        <v>2712</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
@@ -44562,11 +45048,20 @@
       <c r="D11" t="s">
         <v>2451</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="E11" t="s">
+        <v>2793</v>
+      </c>
+      <c r="F11" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G11" t="s">
         <v>2700</v>
+      </c>
+      <c r="H11" t="s">
+        <v>2795</v>
+      </c>
+      <c r="I11" t="s">
+        <v>2794</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -44581,9 +45076,12 @@
         <v>1667</v>
       </c>
       <c r="D12" t="s">
-        <v>1277</v>
-      </c>
-      <c r="F12" s="5" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2797</v>
+      </c>
+      <c r="F12" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G12" t="s">
@@ -44591,11 +45089,10 @@
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>2735</v>
-      </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5" t="s">
-        <v>2737</v>
+        <v>2798</v>
+      </c>
+      <c r="J12" s="94" t="s">
+        <v>2800</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -44611,7 +45108,7 @@
       <c r="D13" t="s">
         <v>2439</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G13" t="s">
@@ -44619,11 +45116,10 @@
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>2736</v>
-      </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5" t="s">
-        <v>2715</v>
+        <v>2729</v>
+      </c>
+      <c r="J13" s="94" t="s">
+        <v>2800</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -44633,24 +45129,27 @@
       <c r="B14" t="s">
         <v>321</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="93" t="s">
         <v>322</v>
       </c>
       <c r="E14" t="s">
         <v>1380</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G14" t="s">
         <v>2700</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K14" s="10"/>
+      <c r="H14" s="94" t="s">
+        <v>2738</v>
+      </c>
+      <c r="I14" s="94" t="s">
+        <v>2739</v>
+      </c>
+      <c r="J14" s="94" t="s">
+        <v>2740</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
@@ -44665,22 +45164,19 @@
       <c r="D15" t="s">
         <v>1713</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G15" t="s">
         <v>2700</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>2716</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>2717</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K15" s="10"/>
+      <c r="H15" s="94" t="s">
+        <v>2713</v>
+      </c>
+      <c r="I15" s="94" t="s">
+        <v>2714</v>
+      </c>
+      <c r="J15" s="94"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
@@ -44695,24 +45191,21 @@
       <c r="E16" t="s">
         <v>1584</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G16" t="s">
         <v>2700</v>
       </c>
-      <c r="H16" s="10" t="s">
-        <v>2718</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>2719</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="H16" s="94" t="s">
+        <v>2715</v>
+      </c>
+      <c r="I16" s="94" t="s">
+        <v>2716</v>
+      </c>
+      <c r="J16" s="94"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>943</v>
       </c>
@@ -44725,49 +45218,45 @@
       <c r="E17" t="s">
         <v>1585</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G17" t="s">
         <v>2700</v>
       </c>
-      <c r="H17" s="10" t="s">
-        <v>2720</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>2721</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="H17" s="94" t="s">
+        <v>2717</v>
+      </c>
+      <c r="I17" s="94" t="s">
+        <v>2718</v>
+      </c>
+      <c r="J17" s="94"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>1081</v>
       </c>
       <c r="B18" t="s">
         <v>1079</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5" t="s">
         <v>1080</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G18" t="s">
         <v>2700</v>
       </c>
       <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10" t="s">
-        <v>1758</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>2714</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="I18" s="5" t="s">
+        <v>2730</v>
+      </c>
+      <c r="J18" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>946</v>
       </c>
@@ -44780,24 +45269,21 @@
       <c r="E19" t="s">
         <v>1586</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G19" t="s">
         <v>2700</v>
       </c>
-      <c r="H19" s="10" t="s">
-        <v>2722</v>
-      </c>
-      <c r="I19" s="10" t="s">
+      <c r="H19" s="94" t="s">
+        <v>2719</v>
+      </c>
+      <c r="I19" s="94" t="s">
         <v>945</v>
       </c>
-      <c r="J19" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>2516</v>
       </c>
@@ -44810,17 +45296,21 @@
       <c r="D20" t="s">
         <v>2454</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G20" t="s">
         <v>2700</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="H20" s="94" t="s">
+        <v>2731</v>
+      </c>
+      <c r="I20" s="94" t="s">
+        <v>2732</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>2527</v>
       </c>
@@ -44830,321 +45320,366 @@
       <c r="C21" t="s">
         <v>1240</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="5" t="s">
         <v>2461</v>
       </c>
       <c r="E21" t="s">
         <v>1719</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G21" t="s">
         <v>2700</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="I21" s="5" t="s">
+        <v>2733</v>
+      </c>
+      <c r="J21" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>2550</v>
       </c>
       <c r="B22" t="s">
         <v>1628</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="93" t="s">
         <v>1089</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="45" t="s">
         <v>1758</v>
       </c>
       <c r="G22" t="s">
         <v>2700</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="J22" s="118" t="s">
+        <v>2741</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>964</v>
       </c>
       <c r="B23" t="s">
         <v>962</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="93" t="s">
         <v>2694</v>
       </c>
       <c r="E23" t="s">
         <v>1592</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="45" t="s">
         <v>1774</v>
       </c>
       <c r="G23" t="s">
         <v>2700</v>
       </c>
-      <c r="J23" s="11" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="H23" t="s">
+        <v>2734</v>
+      </c>
+      <c r="I23" t="s">
+        <v>2735</v>
+      </c>
+      <c r="J23" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>2548</v>
       </c>
       <c r="B24" t="s">
         <v>1629</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="113" t="s">
         <v>43</v>
       </c>
       <c r="E24" t="s">
         <v>1256</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G24" t="s">
         <v>2700</v>
       </c>
-      <c r="J24" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="J24" s="119" t="s">
+        <v>2814</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>53</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="117" t="s">
         <v>52</v>
       </c>
       <c r="E25" t="s">
         <v>1262</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G25" t="s">
         <v>2700</v>
       </c>
-      <c r="J25" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="I25" t="s">
+        <v>2749</v>
+      </c>
+      <c r="J25" t="s">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>59</v>
       </c>
       <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="113" t="s">
         <v>58</v>
       </c>
       <c r="E26" t="s">
         <v>1266</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G26" t="s">
         <v>2700</v>
       </c>
-      <c r="J26" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="H26" t="s">
+        <v>2743</v>
+      </c>
+      <c r="I26" t="s">
+        <v>2744</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>62</v>
       </c>
       <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="113" t="s">
         <v>61</v>
       </c>
       <c r="E27" t="s">
         <v>1268</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G27" t="s">
         <v>2700</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="H27" t="s">
+        <v>2746</v>
+      </c>
+      <c r="I27" t="s">
+        <v>2745</v>
+      </c>
+      <c r="J27" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>71</v>
       </c>
       <c r="B28" t="s">
         <v>69</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="113" t="s">
         <v>70</v>
       </c>
       <c r="E28" t="s">
         <v>1274</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G28" t="s">
         <v>2700</v>
       </c>
-      <c r="J28" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="H28" t="s">
+        <v>2748</v>
+      </c>
+      <c r="I28" t="s">
+        <v>2747</v>
+      </c>
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>74</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="113" t="s">
         <v>73</v>
       </c>
       <c r="E29" t="s">
         <v>1276</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G29" t="s">
         <v>2700</v>
       </c>
-      <c r="J29" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="H29" t="s">
+        <v>2736</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1277</v>
+      </c>
+      <c r="J29" t="s">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>83</v>
       </c>
       <c r="B30" t="s">
         <v>81</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="113" t="s">
         <v>82</v>
       </c>
       <c r="E30" t="s">
         <v>1282</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G30" t="s">
-        <v>2700</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>2801</v>
+      </c>
+      <c r="H30" t="s">
+        <v>2751</v>
+      </c>
+      <c r="I30" t="s">
+        <v>2752</v>
+      </c>
+      <c r="J30" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>1078</v>
       </c>
       <c r="B31" t="s">
         <v>1076</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="117" t="s">
         <v>1077</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G31" t="s">
         <v>2700</v>
       </c>
-      <c r="J31" s="10" t="s">
-        <v>1758</v>
-      </c>
-      <c r="K31" s="10" t="s">
-        <v>2714</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="I31" t="s">
+        <v>2753</v>
+      </c>
+      <c r="J31" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>110</v>
       </c>
       <c r="B32" t="s">
         <v>108</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="113" t="s">
         <v>109</v>
       </c>
       <c r="E32" t="s">
         <v>1300</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G32" t="s">
         <v>2700</v>
       </c>
-      <c r="J32" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K32" s="10"/>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="H32" t="s">
+        <v>2754</v>
+      </c>
+      <c r="I32" t="s">
+        <v>2755</v>
+      </c>
+      <c r="J32" s="94" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>2547</v>
       </c>
       <c r="B33" t="s">
         <v>1635</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="113" t="s">
         <v>121</v>
       </c>
       <c r="E33" t="s">
         <v>1308</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G33" t="s">
         <v>2700</v>
       </c>
-      <c r="J33" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K33" s="10"/>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>137</v>
       </c>
       <c r="B34" t="s">
         <v>135</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="113" t="s">
         <v>136</v>
       </c>
       <c r="E34" t="s">
         <v>1318</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G34" t="s">
-        <v>2700</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>2801</v>
+      </c>
+      <c r="I34" t="s">
+        <v>2757</v>
+      </c>
+      <c r="J34" s="94" t="s">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>2551</v>
       </c>
@@ -45152,19 +45687,17 @@
         <v>1736</v>
       </c>
       <c r="D35" t="s">
-        <v>1236</v>
-      </c>
-      <c r="F35" s="10" t="s">
+        <v>1737</v>
+      </c>
+      <c r="F35" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G35" t="s">
         <v>2700</v>
       </c>
-      <c r="J35" s="10" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="J35" s="10"/>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>2518</v>
       </c>
@@ -45174,60 +45707,62 @@
       <c r="C36" t="s">
         <v>1671</v>
       </c>
-      <c r="D36" t="s">
-        <v>2692</v>
-      </c>
-      <c r="F36" s="10" t="s">
+      <c r="D36" s="5" t="s">
+        <v>2802</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F36" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G36" t="s">
         <v>2700</v>
       </c>
-      <c r="J36" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="I36" s="5" t="s">
+        <v>2804</v>
+      </c>
+      <c r="J36" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>2521</v>
       </c>
       <c r="B37" t="s">
         <v>2609</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="127" t="s">
         <v>1180</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G37" t="s">
         <v>2700</v>
       </c>
-      <c r="J37" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="J37" s="10"/>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>2522</v>
       </c>
       <c r="B38" t="s">
         <v>2610</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="127" t="s">
         <v>1196</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G38" t="s">
         <v>2700</v>
       </c>
-      <c r="J38" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="J38" s="10"/>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>2520</v>
       </c>
@@ -45237,20 +45772,27 @@
       <c r="C39" t="s">
         <v>1210</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="94" t="s">
         <v>2456</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="E39" t="s">
+        <v>2805</v>
+      </c>
+      <c r="F39" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G39" t="s">
         <v>2700</v>
       </c>
-      <c r="J39" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="H39" t="s">
+        <v>2806</v>
+      </c>
+      <c r="I39" t="s">
+        <v>2807</v>
+      </c>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>2519</v>
       </c>
@@ -45260,20 +45802,26 @@
       <c r="C40" t="s">
         <v>1188</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="5" t="s">
         <v>2455</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="E40" t="s">
+        <v>2808</v>
+      </c>
+      <c r="F40" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G40" t="s">
         <v>2700</v>
       </c>
-      <c r="J40" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="I40" t="s">
+        <v>2809</v>
+      </c>
+      <c r="J40" s="94" t="s">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>2529</v>
       </c>
@@ -45283,20 +45831,23 @@
       <c r="C41" t="s">
         <v>1200</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="5" t="s">
         <v>2463</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G41" t="s">
         <v>2700</v>
       </c>
-      <c r="J41" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="I41" s="5" t="s">
+        <v>2758</v>
+      </c>
+      <c r="J41" s="94" t="s">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>2530</v>
       </c>
@@ -45306,43 +45857,49 @@
       <c r="C42" t="s">
         <v>1214</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="5" t="s">
         <v>2464</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G42" t="s">
         <v>2700</v>
       </c>
-      <c r="J42" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="I42" s="5" t="s">
+        <v>2759</v>
+      </c>
+      <c r="J42" s="94" t="s">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>14</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E43" t="s">
         <v>1255</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G43" t="s">
         <v>2700</v>
       </c>
-      <c r="J43" s="10" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="I43" s="5" t="s">
+        <v>2764</v>
+      </c>
+      <c r="J43" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>2531</v>
       </c>
@@ -45352,20 +45909,23 @@
       <c r="C44" t="s">
         <v>1206</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="5" t="s">
         <v>2465</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G44" t="s">
         <v>2700</v>
       </c>
-      <c r="J44" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="I44" s="5" t="s">
+        <v>2762</v>
+      </c>
+      <c r="J44" s="94" t="s">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>2532</v>
       </c>
@@ -45375,20 +45935,23 @@
       <c r="C45" t="s">
         <v>1254</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="5" t="s">
         <v>2466</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G45" t="s">
         <v>2700</v>
       </c>
-      <c r="J45" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="I45" s="5" t="s">
+        <v>2763</v>
+      </c>
+      <c r="J45" s="94" t="s">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>2523</v>
       </c>
@@ -45398,25 +45961,27 @@
       <c r="C46" t="s">
         <v>1244</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="5" t="s">
         <v>2457</v>
       </c>
       <c r="E46" t="s">
         <v>1716</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G46" t="s">
         <v>2700</v>
       </c>
       <c r="H46" s="5"/>
-      <c r="J46" s="5" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K46" s="5"/>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="I46" s="5" t="s">
+        <v>2766</v>
+      </c>
+      <c r="J46" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>2524</v>
       </c>
@@ -45426,25 +45991,27 @@
       <c r="C47" t="s">
         <v>1186</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="5" t="s">
         <v>2458</v>
       </c>
       <c r="E47" t="s">
         <v>1717</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G47" t="s">
         <v>2700</v>
       </c>
       <c r="H47" s="5"/>
-      <c r="J47" s="5" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K47" s="5"/>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="I47" s="5" t="s">
+        <v>2765</v>
+      </c>
+      <c r="J47" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>2525</v>
       </c>
@@ -45454,75 +46021,75 @@
       <c r="C48" t="s">
         <v>1232</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="5" t="s">
         <v>2459</v>
       </c>
       <c r="E48" t="s">
         <v>1718</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G48" t="s">
         <v>2700</v>
       </c>
       <c r="H48" s="5"/>
-      <c r="J48" s="5" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K48" s="5"/>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="I48" s="5" t="s">
+        <v>2767</v>
+      </c>
+      <c r="J48" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>572</v>
       </c>
       <c r="B49" t="s">
         <v>570</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="5" t="s">
         <v>571</v>
       </c>
       <c r="E49" t="s">
         <v>1462</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G49" t="s">
         <v>2700</v>
       </c>
       <c r="H49" s="10"/>
-      <c r="J49" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K49" s="10" t="s">
-        <v>2714</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="I49" t="s">
+        <v>2768</v>
+      </c>
+      <c r="J49" s="119" t="s">
+        <v>2769</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>2534</v>
       </c>
       <c r="B50" t="s">
         <v>2622</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="128" t="s">
         <v>1689</v>
       </c>
       <c r="E50" t="s">
         <v>2691</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G50" t="s">
         <v>2700</v>
       </c>
-      <c r="J50" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="J50" s="10"/>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>2535</v>
       </c>
@@ -45532,40 +46099,43 @@
       <c r="C51" t="s">
         <v>1228</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="5" t="s">
         <v>2467</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G51" t="s">
         <v>2700</v>
       </c>
-      <c r="J51" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="J51" s="119" t="s">
+        <v>2770</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>2579</v>
       </c>
       <c r="B52" t="s">
         <v>2657</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="5" t="s">
         <v>1160</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G52" t="s">
         <v>2700</v>
       </c>
-      <c r="J52" s="10" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="I52" s="5" t="s">
+        <v>2772</v>
+      </c>
+      <c r="J52" s="94" t="s">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>2580</v>
       </c>
@@ -45575,17 +46145,21 @@
       <c r="D53" t="s">
         <v>1148</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G53" t="s">
         <v>2700</v>
       </c>
-      <c r="J53" s="10" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="H53" t="s">
+        <v>2771</v>
+      </c>
+      <c r="I53" t="s">
+        <v>1148</v>
+      </c>
+      <c r="J53" s="10"/>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>2536</v>
       </c>
@@ -45595,20 +46169,26 @@
       <c r="C54" t="s">
         <v>1182</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="5" t="s">
         <v>2468</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="E54" t="s">
+        <v>2810</v>
+      </c>
+      <c r="F54" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G54" t="s">
         <v>2700</v>
       </c>
-      <c r="J54" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="I54" s="5" t="s">
+        <v>2812</v>
+      </c>
+      <c r="J54" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>2537</v>
       </c>
@@ -45621,40 +46201,47 @@
       <c r="D55" t="s">
         <v>2470</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="E55" t="s">
+        <v>2811</v>
+      </c>
+      <c r="F55" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G55" t="s">
         <v>2700</v>
       </c>
-      <c r="J55" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="H55" t="s">
+        <v>2774</v>
+      </c>
+      <c r="I55" t="s">
+        <v>2775</v>
+      </c>
+      <c r="J55" s="94" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>2496</v>
       </c>
       <c r="B56" t="s">
         <v>1751</v>
       </c>
-      <c r="C56" t="b">
+      <c r="C56" s="93" t="b">
         <v>0</v>
       </c>
       <c r="D56" t="s">
         <v>1230</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G56" t="s">
         <v>2700</v>
       </c>
-      <c r="J56" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>2538</v>
       </c>
@@ -45664,38 +46251,38 @@
       <c r="D57" t="s">
         <v>1208</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G57" t="s">
         <v>2700</v>
       </c>
-      <c r="J57" s="5" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>2582</v>
       </c>
       <c r="B58" t="s">
         <v>2660</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="5" t="s">
         <v>1106</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="F58" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G58" t="s">
         <v>2700</v>
       </c>
-      <c r="J58" s="10" t="s">
-        <v>1758</v>
-      </c>
-      <c r="K58" s="10"/>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="I58" s="5" t="s">
+        <v>2776</v>
+      </c>
+      <c r="J58" s="94" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>2539</v>
       </c>
@@ -45705,23 +46292,23 @@
       <c r="C59" t="s">
         <v>1194</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="5" t="s">
         <v>2471</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G59" t="s">
         <v>2700</v>
       </c>
-      <c r="J59" s="5" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K59" s="5" t="s">
-        <v>2723</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="I59" s="5" t="s">
+        <v>2777</v>
+      </c>
+      <c r="J59" s="94" t="s">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>2540</v>
       </c>
@@ -45731,20 +46318,17 @@
       <c r="D60" t="s">
         <v>1252</v>
       </c>
-      <c r="F60" s="10" t="s">
+      <c r="F60" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G60" t="s">
         <v>2700</v>
       </c>
-      <c r="J60" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K60" s="10" t="s">
-        <v>2724</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="J60" s="120" t="s">
+        <v>2720</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>2541</v>
       </c>
@@ -45754,26 +46338,21 @@
       <c r="D61" t="s">
         <v>1198</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F61" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G61" t="s">
         <v>2700</v>
       </c>
-      <c r="H61" s="10" t="s">
-        <v>2726</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>2727</v>
-      </c>
-      <c r="J61" s="10" t="s">
-        <v>1774</v>
-      </c>
-      <c r="K61" s="10" t="s">
-        <v>2725</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="H61" s="94" t="s">
+        <v>2721</v>
+      </c>
+      <c r="I61" s="94" t="s">
+        <v>2722</v>
+      </c>
+      <c r="J61" s="120"/>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>901</v>
       </c>
@@ -45786,17 +46365,15 @@
       <c r="E62" t="s">
         <v>1572</v>
       </c>
-      <c r="F62" s="10" t="s">
+      <c r="F62" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G62" t="s">
         <v>2700</v>
       </c>
-      <c r="J62" s="10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="J62" s="10"/>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>2504</v>
       </c>
@@ -45809,23 +46386,23 @@
       <c r="D63" t="s">
         <v>2450</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G63" t="s">
         <v>2700</v>
       </c>
-      <c r="H63" t="s">
-        <v>2708</v>
-      </c>
-      <c r="J63" t="s">
+      <c r="H63" s="94" t="s">
         <v>2707</v>
       </c>
-      <c r="K63" t="s">
-        <v>2709</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="I63" t="s">
+        <v>2706</v>
+      </c>
+      <c r="J63" s="121" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>2528</v>
       </c>
@@ -45838,20 +46415,20 @@
       <c r="D64" t="s">
         <v>2462</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G64" t="s">
         <v>2700</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="94" t="s">
+        <v>2703</v>
+      </c>
+      <c r="I64" t="s">
         <v>2704</v>
       </c>
-      <c r="K64" t="s">
-        <v>2703</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>2526</v>
       </c>
@@ -45861,17 +46438,17 @@
       <c r="D65" t="s">
         <v>1216</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G65" t="s">
         <v>2700</v>
       </c>
-      <c r="J65" t="s">
-        <v>2710</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="I65" t="s">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>2555</v>
       </c>
@@ -45881,63 +46458,63 @@
       <c r="D66" t="s">
         <v>1155</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G66" t="s">
         <v>2700</v>
       </c>
-      <c r="J66" t="s">
-        <v>2705</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>1033</v>
       </c>
       <c r="B67" t="s">
         <v>1031</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="5" t="s">
         <v>1032</v>
       </c>
       <c r="E67" t="s">
         <v>1614</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G67" t="s">
         <v>2700</v>
       </c>
+      <c r="I67" s="5" t="s">
+        <v>2779</v>
+      </c>
       <c r="J67" t="s">
-        <v>2706</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>1075</v>
       </c>
       <c r="B68" t="s">
         <v>1073</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="5" t="s">
         <v>1074</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="94" t="s">
         <v>1758</v>
       </c>
       <c r="G68" t="s">
         <v>2700</v>
       </c>
+      <c r="I68" s="5" t="s">
+        <v>2702</v>
+      </c>
       <c r="J68" t="s">
         <v>2701</v>
       </c>
-      <c r="K68" t="s">
-        <v>2702</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>2546</v>
       </c>
@@ -45950,17 +46527,14 @@
       <c r="D69" t="s">
         <v>2469</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="94" t="s">
         <v>1774</v>
       </c>
       <c r="G69" t="s">
         <v>2700</v>
       </c>
-      <c r="J69" t="s">
-        <v>2705</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -45973,11 +46547,11 @@
       <c r="E70" t="s">
         <v>1322</v>
       </c>
-      <c r="F70" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="F70" s="94" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>2497</v>
       </c>
@@ -45988,7 +46562,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>2501</v>
       </c>
@@ -45999,7 +46573,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>910</v>
       </c>
@@ -46016,7 +46590,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -46033,7 +46607,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>2544</v>
       </c>
@@ -46044,7 +46618,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>149</v>
       </c>
@@ -46061,7 +46635,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -46078,7 +46652,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>161</v>
       </c>
@@ -46095,7 +46669,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>164</v>
       </c>
@@ -46112,7 +46686,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -47178,7 +47752,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:10">
       <c r="A145" t="s">
         <v>311</v>
       </c>
@@ -47195,7 +47769,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:10">
       <c r="A146" t="s">
         <v>314</v>
       </c>
@@ -47212,7 +47786,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:10">
       <c r="A147" t="s">
         <v>317</v>
       </c>
@@ -47229,7 +47803,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:10">
       <c r="A148" t="s">
         <v>320</v>
       </c>
@@ -47246,7 +47820,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="149" spans="1:11">
+    <row r="149" spans="1:10">
       <c r="A149" t="s">
         <v>326</v>
       </c>
@@ -47266,9 +47840,8 @@
       <c r="H149" s="10"/>
       <c r="I149" s="10"/>
       <c r="J149" s="10"/>
-      <c r="K149" s="10"/>
-    </row>
-    <row r="150" spans="1:11">
+    </row>
+    <row r="150" spans="1:10">
       <c r="A150" t="s">
         <v>329</v>
       </c>
@@ -47288,9 +47861,8 @@
       <c r="H150" s="10"/>
       <c r="I150" s="10"/>
       <c r="J150" s="10"/>
-      <c r="K150" s="10"/>
-    </row>
-    <row r="151" spans="1:11">
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151" t="s">
         <v>332</v>
       </c>
@@ -47310,9 +47882,8 @@
       <c r="H151" s="10"/>
       <c r="I151" s="10"/>
       <c r="J151" s="10"/>
-      <c r="K151" s="10"/>
-    </row>
-    <row r="152" spans="1:11">
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152" t="s">
         <v>937</v>
       </c>
@@ -47332,9 +47903,8 @@
       <c r="H152" s="10"/>
       <c r="I152" s="10"/>
       <c r="J152" s="10"/>
-      <c r="K152" s="10"/>
-    </row>
-    <row r="153" spans="1:11">
+    </row>
+    <row r="153" spans="1:10">
       <c r="A153" t="s">
         <v>952</v>
       </c>
@@ -47351,7 +47921,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:10">
       <c r="A154" t="s">
         <v>955</v>
       </c>
@@ -47368,7 +47938,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:10">
       <c r="A155" t="s">
         <v>958</v>
       </c>
@@ -47385,7 +47955,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:10">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -47402,7 +47972,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:10">
       <c r="A157" t="s">
         <v>158</v>
       </c>
@@ -47419,7 +47989,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:10">
       <c r="A158" t="s">
         <v>398</v>
       </c>
@@ -47436,7 +48006,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:10">
       <c r="A159" t="s">
         <v>401</v>
       </c>
@@ -47453,7 +48023,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:10">
       <c r="A160" t="s">
         <v>338</v>
       </c>
@@ -48004,7 +48574,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" spans="1:10">
       <c r="A193" t="s">
         <v>410</v>
       </c>
@@ -48021,7 +48591,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="194" spans="1:11">
+    <row r="194" spans="1:10">
       <c r="A194" t="s">
         <v>47</v>
       </c>
@@ -48040,7 +48610,7 @@
       <c r="G194" s="10"/>
       <c r="J194" s="10"/>
     </row>
-    <row r="195" spans="1:11">
+    <row r="195" spans="1:10">
       <c r="A195" t="s">
         <v>50</v>
       </c>
@@ -48059,7 +48629,7 @@
       <c r="G195" s="10"/>
       <c r="J195" s="10"/>
     </row>
-    <row r="196" spans="1:11">
+    <row r="196" spans="1:10">
       <c r="A196" t="s">
         <v>65</v>
       </c>
@@ -48078,7 +48648,7 @@
       <c r="G196" s="10"/>
       <c r="J196" s="10"/>
     </row>
-    <row r="197" spans="1:11">
+    <row r="197" spans="1:10">
       <c r="A197" t="s">
         <v>56</v>
       </c>
@@ -48097,7 +48667,7 @@
       <c r="G197" s="10"/>
       <c r="J197" s="10"/>
     </row>
-    <row r="198" spans="1:11">
+    <row r="198" spans="1:10">
       <c r="A198" t="s">
         <v>68</v>
       </c>
@@ -48116,7 +48686,7 @@
       <c r="G198" s="10"/>
       <c r="J198" s="10"/>
     </row>
-    <row r="199" spans="1:11">
+    <row r="199" spans="1:10">
       <c r="A199" t="s">
         <v>77</v>
       </c>
@@ -48135,7 +48705,7 @@
       <c r="G199" s="10"/>
       <c r="J199" s="10"/>
     </row>
-    <row r="200" spans="1:11">
+    <row r="200" spans="1:10">
       <c r="A200" t="s">
         <v>80</v>
       </c>
@@ -48154,7 +48724,7 @@
       <c r="G200" s="10"/>
       <c r="J200" s="10"/>
     </row>
-    <row r="201" spans="1:11">
+    <row r="201" spans="1:10">
       <c r="A201" t="s">
         <v>86</v>
       </c>
@@ -48171,7 +48741,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="202" spans="1:11">
+    <row r="202" spans="1:10">
       <c r="A202" t="s">
         <v>89</v>
       </c>
@@ -48188,7 +48758,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="203" spans="1:11">
+    <row r="203" spans="1:10">
       <c r="A203" t="s">
         <v>92</v>
       </c>
@@ -48205,7 +48775,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="204" spans="1:11">
+    <row r="204" spans="1:10">
       <c r="A204" t="s">
         <v>95</v>
       </c>
@@ -48222,7 +48792,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" spans="1:10">
       <c r="A205" t="s">
         <v>98</v>
       </c>
@@ -48240,9 +48810,8 @@
       </c>
       <c r="G205" s="10"/>
       <c r="J205" s="10"/>
-      <c r="K205" s="10"/>
-    </row>
-    <row r="206" spans="1:11">
+    </row>
+    <row r="206" spans="1:10">
       <c r="A206" t="s">
         <v>101</v>
       </c>
@@ -48260,9 +48829,8 @@
       </c>
       <c r="G206" s="10"/>
       <c r="J206" s="10"/>
-      <c r="K206" s="10"/>
-    </row>
-    <row r="207" spans="1:11">
+    </row>
+    <row r="207" spans="1:10">
       <c r="A207" t="s">
         <v>104</v>
       </c>
@@ -48280,9 +48848,8 @@
       </c>
       <c r="G207" s="10"/>
       <c r="J207" s="10"/>
-      <c r="K207" s="10"/>
-    </row>
-    <row r="208" spans="1:11">
+    </row>
+    <row r="208" spans="1:10">
       <c r="A208" t="s">
         <v>107</v>
       </c>
@@ -48300,9 +48867,8 @@
       </c>
       <c r="G208" s="10"/>
       <c r="J208" s="10"/>
-      <c r="K208" s="10"/>
-    </row>
-    <row r="209" spans="1:11">
+    </row>
+    <row r="209" spans="1:10">
       <c r="A209" t="s">
         <v>113</v>
       </c>
@@ -48320,9 +48886,8 @@
       </c>
       <c r="G209" s="10"/>
       <c r="J209" s="10"/>
-      <c r="K209" s="10"/>
-    </row>
-    <row r="210" spans="1:11">
+    </row>
+    <row r="210" spans="1:10">
       <c r="A210" t="s">
         <v>116</v>
       </c>
@@ -48340,9 +48905,8 @@
       </c>
       <c r="G210" s="10"/>
       <c r="J210" s="10"/>
-      <c r="K210" s="10"/>
-    </row>
-    <row r="211" spans="1:11">
+    </row>
+    <row r="211" spans="1:10">
       <c r="A211" t="s">
         <v>119</v>
       </c>
@@ -48360,9 +48924,8 @@
       </c>
       <c r="G211" s="10"/>
       <c r="J211" s="10"/>
-      <c r="K211" s="10"/>
-    </row>
-    <row r="212" spans="1:11">
+    </row>
+    <row r="212" spans="1:10">
       <c r="A212" t="s">
         <v>125</v>
       </c>
@@ -48379,7 +48942,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="213" spans="1:11">
+    <row r="213" spans="1:10">
       <c r="A213" t="s">
         <v>970</v>
       </c>
@@ -48396,7 +48959,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="214" spans="1:11">
+    <row r="214" spans="1:10">
       <c r="A214" t="s">
         <v>128</v>
       </c>
@@ -48413,7 +48976,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="215" spans="1:11">
+    <row r="215" spans="1:10">
       <c r="A215" t="s">
         <v>131</v>
       </c>
@@ -48430,7 +48993,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:10">
       <c r="A216" t="s">
         <v>134</v>
       </c>
@@ -48447,7 +49010,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="217" spans="1:11">
+    <row r="217" spans="1:10">
       <c r="A217" t="s">
         <v>140</v>
       </c>
@@ -48466,7 +49029,7 @@
       <c r="G217" s="10"/>
       <c r="J217" s="10"/>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" spans="1:10">
       <c r="A218" t="s">
         <v>413</v>
       </c>
@@ -48483,7 +49046,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="219" spans="1:11">
+    <row r="219" spans="1:10">
       <c r="A219" t="s">
         <v>416</v>
       </c>
@@ -48500,7 +49063,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" spans="1:10">
       <c r="A220" t="s">
         <v>419</v>
       </c>
@@ -48517,7 +49080,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="221" spans="1:11">
+    <row r="221" spans="1:10">
       <c r="A221" t="s">
         <v>422</v>
       </c>
@@ -48534,7 +49097,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:10">
       <c r="A222" t="s">
         <v>425</v>
       </c>
@@ -48551,7 +49114,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="223" spans="1:11">
+    <row r="223" spans="1:10">
       <c r="A223" t="s">
         <v>428</v>
       </c>
@@ -48568,7 +49131,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="224" spans="1:11">
+    <row r="224" spans="1:10">
       <c r="A224" t="s">
         <v>431</v>
       </c>
@@ -52233,56 +52796,175 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="40.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>2728</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:4">
+      <c r="A1" s="19" t="s">
+        <v>2723</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1226</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>2729</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
+      <c r="D2" s="124" t="s">
+        <v>2788</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D3" s="124" t="s">
+        <v>2789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D4" s="124" t="s">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18">
+      <c r="A8" s="116" t="s">
+        <v>2724</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>1709</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
+      <c r="B9" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>2449</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+      <c r="B10" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>2693</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
         <v>2451</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
+      <c r="B12" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>1277</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
+      <c r="B13" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>2439</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>2456</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>2455</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>2468</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>2470</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="119" t="s">
+        <v>2813</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add missing website for ENVO ontology
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@80293 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/Microbiome/doc/microbiome_terms.xlsx
+++ b/Load/src/ontology/Microbiome/doc/microbiome_terms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="160" windowWidth="25360" windowHeight="13920" tabRatio="775" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="6240" yWindow="320" windowWidth="25600" windowHeight="16060" tabRatio="775" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="IRI mappings(webProtege)" sheetId="13" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="ontology mapping" sheetId="16" r:id="rId7"/>
     <sheet name="ToDo in ontology" sheetId="17" r:id="rId8"/>
     <sheet name="Penn DataSet" sheetId="15" r:id="rId9"/>
+    <sheet name="annotationUpdates" sheetId="18" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11721" uniqueCount="3040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11895" uniqueCount="3043">
   <si>
     <t>Name</t>
   </si>
@@ -9165,12 +9166,21 @@
   <si>
     <t>Child's diet (by month)</t>
   </si>
+  <si>
+    <t>IRI</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/01/rdf-schema#label</t>
+  </si>
+  <si>
+    <t>Environmental feature level includes geographic environmental features. Compared to biome, feature is a descriptor of the more local environment. Examples include: harbor, cliff, or lake. EnvO (v 2013-06-14) terms can be found via the link: www.environmentontology.org</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="54" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -9541,6 +9551,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -9926,7 +9942,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="495">
+  <cellStyleXfs count="498">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -10422,8 +10438,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -10555,8 +10574,9 @@
     <xf numFmtId="0" fontId="24" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="495">
+  <cellStyles count="498">
     <cellStyle name="20% - Accent1" xfId="208" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="212" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="216" builtinId="38" customBuiltin="1"/>
@@ -11028,6 +11048,9 @@
     <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="497" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="196" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="192" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="193" builtinId="17" customBuiltin="1"/>
@@ -12685,6 +12708,719 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="48.83203125" customWidth="1"/>
+    <col min="2" max="3" width="58.33203125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18">
+      <c r="A1" t="s">
+        <v>3040</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>3041</v>
+      </c>
+      <c r="C1" s="129" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>2500</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>2509</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>2503</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>2449</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>2499</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2447</v>
+      </c>
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>2510</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>2505</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>2784</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>2507</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>2451</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2792</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>2513</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>2795</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>2512</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>3039</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>2517</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>940</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>939</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>943</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>942</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C17"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>946</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>2454</v>
+      </c>
+      <c r="C19"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>2527</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>2550</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C21"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>964</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>2694</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>2548</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C30"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>2551</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C34"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>2518</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>2801</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2802</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>2521</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>2522</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>2520</v>
+      </c>
+      <c r="B38" s="45" t="s">
+        <v>2456</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2804</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>2519</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>2455</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2807</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>2529</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>2463</v>
+      </c>
+      <c r="C40"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>2530</v>
+      </c>
+      <c r="B41" s="42" t="s">
+        <v>2464</v>
+      </c>
+      <c r="C41"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>2531</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>2465</v>
+      </c>
+      <c r="C43"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>2532</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>2466</v>
+      </c>
+      <c r="C44"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>2523</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>2457</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>2524</v>
+      </c>
+      <c r="B46" s="42" t="s">
+        <v>2458</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>2525</v>
+      </c>
+      <c r="B47" s="42" t="s">
+        <v>2459</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>572</v>
+      </c>
+      <c r="B48" s="42" t="s">
+        <v>571</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>2534</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2691</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>2535</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>2467</v>
+      </c>
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>2579</v>
+      </c>
+      <c r="B51" s="42" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>2580</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>2536</v>
+      </c>
+      <c r="B53" s="42" t="s">
+        <v>2468</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>2537</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>2496</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>2538</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>2582</v>
+      </c>
+      <c r="B57" s="42" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C57"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>2539</v>
+      </c>
+      <c r="B58" s="42" t="s">
+        <v>2471</v>
+      </c>
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>2540</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C59"/>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>2541</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C60"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>901</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>2504</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C62"/>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>2528</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>2462</v>
+      </c>
+      <c r="C63"/>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>2526</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C64"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>2555</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C65"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B66" s="42" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B67" s="42" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C67"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>2546</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>2469</v>
+      </c>
+      <c r="C68"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC452"/>
@@ -45512,8 +46248,8 @@
   <dimension ref="A1:K446"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -45957,7 +46693,7 @@
         <v>942</v>
       </c>
       <c r="E16" t="s">
-        <v>1585</v>
+        <v>3042</v>
       </c>
       <c r="F16" s="94" t="s">
         <v>1774</v>

</xml_diff>